<commit_message>
matlab week 2: almost done with RLE decoder
</commit_message>
<xml_diff>
--- a/matlab_bootcamp/GoL_input.xlsx
+++ b/matlab_bootcamp/GoL_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedar\aether_repo\matlab_bootcamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kedarK 1/aetherrepo/matlab_bootcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967040AE-567E-4AA1-9EB4-EF8F2E33B39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4A2EC9-6012-484D-AEB5-B3DAC04CFA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE56AE60-CC91-4FB8-8B70-FE4A2F09FA22}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{BE56AE60-CC91-4FB8-8B70-FE4A2F09FA22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,10 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,15 +380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCE76DB-ED2E-4E4F-9897-F6890D1DD046}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
@@ -409,20 +404,8 @@
       <c r="E1">
         <v>0</v>
       </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -430,7 +413,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -438,20 +421,8 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -462,54 +433,30 @@
         <v>1</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -520,108 +467,9 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
         <v>0</v>
       </c>
     </row>

</xml_diff>